<commit_message>
loss made pretty 2
</commit_message>
<xml_diff>
--- a/loss.xlsx
+++ b/loss.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,31 +434,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Training</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[0.02688300848007202, 0.0059753404557704925, 0.004181852899491787, 0.0036908319592475892, 0.003413166105747223, 0.003272998631000519, 0.0030285048484802245, 0.0030331866815686225, 0.0027528297528624534, 0.0028411054611206053]</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Validation</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
-          <t>[0.01573835462331772, 0.014160224795341491, 0.02277475818991661, 0.02341669276356697, 0.024950604885816574, 0.01731770932674408, 0.026488222181797028, 0.030340880155563354, 0.02782386541366577, 0.009981201589107513]</t>
+          <t>[0.03761576488614082, 0.007720354124903679, 0.004869405888020992, 0.004016904495656491, 0.003860360607504845, 0.0033066946268081663, 0.003209751956164837, 0.003131478950381279, 0.002889433428645134, 0.002608037553727627]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[4.466980361938477, 0.013171311095356941, 0.013815078884363174, 0.018883594870567323, 0.024239375442266464, 0.022170404344797133, 0.02061031311750412, 0.02529122605919838, 0.02824832797050476, 0.02674718052148819]</t>
         </is>
       </c>
     </row>

</xml_diff>